<commit_message>
Update for Magozzi resub
</commit_message>
<xml_diff>
--- a/data-raw/ham.xlsx
+++ b/data-raw/ham.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sarah/Dropbox/HO_database/paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0133977\Documents\GitHub\assignR\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5337AB95-7965-EF4E-94E7-28DDD35C6F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="13720"/>
   </bookViews>
   <sheets>
     <sheet name="ham" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,33 +36,6 @@
   </si>
   <si>
     <t>DEN_H_2</t>
-  </si>
-  <si>
-    <t>OldSA.1_H_1</t>
-  </si>
-  <si>
-    <t>OldSA.2_H_1</t>
-  </si>
-  <si>
-    <t>SA_H_1</t>
-  </si>
-  <si>
-    <t>SA_H_2</t>
-  </si>
-  <si>
-    <t>SA_H_3</t>
-  </si>
-  <si>
-    <t>SA_H_4</t>
-  </si>
-  <si>
-    <t>SA_H_5</t>
-  </si>
-  <si>
-    <t>SA_H_6</t>
-  </si>
-  <si>
-    <t>SA_H_7</t>
   </si>
   <si>
     <t>OldUT_H_1</t>
@@ -132,16 +104,43 @@
     <t>VSMOW_H</t>
   </si>
   <si>
-    <t>SA_H_8</t>
+    <t>OldEC.1_H_1</t>
   </si>
   <si>
-    <t>SA_H_9</t>
+    <t>OldEC.2_H_1</t>
+  </si>
+  <si>
+    <t>EC_H_1</t>
+  </si>
+  <si>
+    <t>EC_H_2</t>
+  </si>
+  <si>
+    <t>EC_H_3</t>
+  </si>
+  <si>
+    <t>EC_H_4</t>
+  </si>
+  <si>
+    <t>EC_H_5</t>
+  </si>
+  <si>
+    <t>EC_H_6</t>
+  </si>
+  <si>
+    <t>EC_H_7</t>
+  </si>
+  <si>
+    <t>EC_H_8</t>
+  </si>
+  <si>
+    <t>EC_H_9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -200,7 +199,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -511,14 +510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="16384" width="12.83203125" style="1"/>
   </cols>
@@ -531,31 +530,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>33</v>
@@ -564,70 +563,70 @@
         <v>34</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Z1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AG1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AH1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AI1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:36">
@@ -852,7 +851,7 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -962,7 +961,7 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1072,7 +1071,7 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -1182,7 +1181,7 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1292,7 +1291,7 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1402,7 +1401,7 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1512,7 +1511,7 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1622,7 +1621,7 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -1732,7 +1731,7 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -2062,7 +2061,7 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -2172,7 +2171,7 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -2282,7 +2281,7 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -2392,7 +2391,7 @@
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -2502,7 +2501,7 @@
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -2612,7 +2611,7 @@
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -2722,7 +2721,7 @@
     </row>
     <row r="21" spans="1:36">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -2832,7 +2831,7 @@
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -2942,7 +2941,7 @@
     </row>
     <row r="23" spans="1:36">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -3052,7 +3051,7 @@
     </row>
     <row r="24" spans="1:36">
       <c r="A24" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -3162,7 +3161,7 @@
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -3272,7 +3271,7 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -3382,7 +3381,7 @@
     </row>
     <row r="27" spans="1:36">
       <c r="A27" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -3492,7 +3491,7 @@
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -3602,7 +3601,7 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -3712,7 +3711,7 @@
     </row>
     <row r="30" spans="1:36">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -3822,7 +3821,7 @@
     </row>
     <row r="31" spans="1:36">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -3932,7 +3931,7 @@
     </row>
     <row r="32" spans="1:36">
       <c r="A32" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -4042,7 +4041,7 @@
     </row>
     <row r="33" spans="1:36">
       <c r="A33" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -4152,7 +4151,7 @@
     </row>
     <row r="34" spans="1:36">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -4262,7 +4261,7 @@
     </row>
     <row r="35" spans="1:36">
       <c r="A35" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -4372,7 +4371,7 @@
     </row>
     <row r="36" spans="1:36">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>

</xml_diff>